<commit_message>
add excel , last experimentos
</commit_message>
<xml_diff>
--- a/heuristico_time.xlsx
+++ b/heuristico_time.xlsx
@@ -1,50 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csierra\AppData\Local\Temp\BvSshSftp-WQNJVJUV\LRG7K3N1\448ATCL5\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992A24C2-CB5B-481A-A9C5-4B136B59F296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,23 +45,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -378,56 +419,750 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="55.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:06</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>0.383842945098877</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:11</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.05684471130371094</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:15</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.08631253242492676</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:19</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.08617734909057617</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.06531977653503418</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:36</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.08761453628540039</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:44</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.08604884147644043</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:48</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.05626535415649414</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:22:53</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1163454055786133</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:03</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.08728909492492676</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.06247901916503906</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:28</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.08662152290344238</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:33</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.08624672889709473</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:40</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.08703374862670898</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:50</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.05664467811584473</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:23:55</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.08597564697265625</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:24:02</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.05929994583129883</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:24:15</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.05660009384155273</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>input6_heuristic_2024-10-23_08:24:20</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0565645694732666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:29:17</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.37644362449646</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:29:23</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.06214714050292969</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:30:05</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.08993029594421387</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:30:24</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.08647561073303223</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:30:30</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.08668088912963867</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:30:38</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.08928442001342773</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:06</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.08610177040100098</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:12</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.05659961700439453</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:17</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.05802583694458008</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:29</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.05663943290710449</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:35</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.05849599838256836</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:31:52</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.0603644847869873</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:32:34</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.08596110343933105</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:32:41</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.08685111999511719</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:32:50</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.08589792251586914</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:32:57</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.08799362182617188</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:33:09</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.08656811714172363</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>input5_heuristic_2024-10-23_08:33:19</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.1154410839080811</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:37:43</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.4111917018890381</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:38:02</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.1152384281158447</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:38:10</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.08783888816833496</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:38:34</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.08750200271606445</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:38:45</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.05666136741638184</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:38:51</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.08782219886779785</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:39:09</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.08531022071838379</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:39:23</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.05631136894226074</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:39:34</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.05669784545898438</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:39:40</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.05630922317504883</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:39:46</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.08585810661315918</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:40:00</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.05800342559814453</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:40:16</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.08859086036682129</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:40:43</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.1170792579650879</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:41:01</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.05972695350646973</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>input2_heuristic_2024-10-23_08:41:31</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.06578159332275391</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:44:01</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.4113092422485352</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:44:16</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.10272216796875</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:45:13</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.08552122116088867</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:45:21</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.0879511833190918</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:45:42</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.08582496643066406</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:45:49</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.05642437934875488</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:45:56</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.08758783340454102</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:46:19</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.06023240089416504</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:46:54</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.08948302268981934</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:47:36</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.1164600849151611</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:47:54</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.08609294891357422</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:48:04</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.1208477020263672</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:48:55</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.08627891540527344</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:49:06</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.08670401573181152</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:49:24</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.08752322196960449</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:49:40</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.08591079711914062</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:49:49</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.09243893623352051</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:51:05</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0856478214263916</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:51:14</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.05616569519042969</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>input1_heuristic_2024-10-23_08:51:20</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.08630084991455078</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>